<commit_message>
Removed seepage velocity from derived parameters output and simplified plot titles by removing "1D Advection-Diffusion:" prefix
</commit_message>
<xml_diff>
--- a/conc_data.xlsx
+++ b/conc_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jones/python_projects/adsolve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenelson/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C76CFA-A485-9B44-AE6D-256F341BC579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2EC9AB-EE5A-D64E-ACDB-9A08949C5DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="28600" windowHeight="18560" activeTab="2" xr2:uid="{B672A836-5648-D342-817E-0FAB6C4978C8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28600" windowHeight="18560" activeTab="5" xr2:uid="{B672A836-5648-D342-817E-0FAB6C4978C8}"/>
   </bookViews>
   <sheets>
     <sheet name="TSSD" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="DW25" sheetId="3" r:id="rId3"/>
     <sheet name="Diffusion parameters" sheetId="4" r:id="rId4"/>
     <sheet name="Chloride data" sheetId="5" r:id="rId5"/>
+    <sheet name="Orthophosphate data" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="158">
   <si>
     <t>Sample ID</t>
   </si>
@@ -691,7 +692,19 @@
     <t>Filtered field and/or lab</t>
   </si>
   <si>
+    <t>Orthophosphate</t>
+  </si>
+  <si>
     <t>Chloride</t>
+  </si>
+  <si>
+    <t>NAD84</t>
+  </si>
+  <si>
+    <t>NAD85</t>
+  </si>
+  <si>
+    <t>NAD86</t>
   </si>
 </sst>
 </file>
@@ -702,7 +715,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -773,6 +786,12 @@
       <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3621,7 +3640,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.5949973770182186E-2"/>
+          <c:y val="7.5364684664922618E-2"/>
+          <c:w val="0.85960344691362478"/>
+          <c:h val="0.90484936504237001"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -3650,6 +3679,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.18402038214626107"/>
+                  <c:y val="9.3006274171576281E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'DW25'!$Q$2:$Q$27</c:f>
@@ -4193,6 +4272,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.32092104979062414"/>
+                  <c:y val="1.1752854473868212E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'DW25'!$R$2:$R$27</c:f>
@@ -5311,7 +5440,7 @@
                   <c:v>-8.7670038896078459</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.6382721639824069</c:v>
+                  <c:v>-8.6925039620867874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6862,7 +6991,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1600"/>
-              <a:t>P mg/L</a:t>
+              <a:t>P micrograms/L</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -19181,15 +19310,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>35277</xdr:colOff>
+      <xdr:colOff>35276</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>35277</xdr:rowOff>
+      <xdr:rowOff>35278</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>388056</xdr:colOff>
+      <xdr:colOff>388055</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>23519</xdr:rowOff>
+      <xdr:rowOff>23520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19219,15 +19348,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>470371</xdr:colOff>
+      <xdr:colOff>422894</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>35277</xdr:rowOff>
+      <xdr:rowOff>23408</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>329261</xdr:colOff>
+      <xdr:colOff>281784</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>23518</xdr:rowOff>
+      <xdr:rowOff>11649</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19257,15 +19386,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>329259</xdr:colOff>
+      <xdr:colOff>293653</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>35278</xdr:rowOff>
+      <xdr:rowOff>23409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>540927</xdr:colOff>
+      <xdr:colOff>505321</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>23519</xdr:rowOff>
+      <xdr:rowOff>11650</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19434,15 +19563,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>999536</xdr:colOff>
+      <xdr:colOff>963929</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>23519</xdr:rowOff>
+      <xdr:rowOff>35388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>470371</xdr:colOff>
+      <xdr:colOff>434764</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>11761</xdr:rowOff>
+      <xdr:rowOff>23630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19476,16 +19605,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>742950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>425450</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19513,15 +19642,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>711200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19550,16 +19679,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>723900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19589,15 +19718,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>723900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19627,15 +19756,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>749300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19705,16 +19834,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>577273</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>69273</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>104486</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>45605</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19744,15 +19873,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>311727</xdr:colOff>
+      <xdr:colOff>115455</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46181</xdr:rowOff>
+      <xdr:rowOff>80818</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>508578</xdr:colOff>
+      <xdr:colOff>312306</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>22513</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19782,15 +19911,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>531092</xdr:colOff>
+      <xdr:colOff>311728</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>23091</xdr:rowOff>
+      <xdr:rowOff>57727</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>58306</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>207241</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>508579</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>34059</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19819,16 +19948,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>508001</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>46181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>196851</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>35215</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>22513</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20407,8 +20536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D2CECF-4970-6944-97C8-81B0EE7A7087}">
   <dimension ref="A1:AK328"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="107" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42:K50"/>
+    <sheetView topLeftCell="A4" zoomScale="107" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5:Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -35354,8 +35483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D340663C-23C1-EF45-A0DC-1334D29F7354}">
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D20"/>
+    <sheetView topLeftCell="K1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37366,8 +37495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A09E69-E6D4-CC4C-8A80-256D255F91E4}">
   <dimension ref="A1:AL30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39787,8 +39916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8267C9D4-30E8-174D-9514-9D4C98E4DEE4}">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView topLeftCell="D27" zoomScale="109" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q38" sqref="Q38"/>
+    <sheetView topLeftCell="A21" zoomScale="109" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34:T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40027,18 +40156,18 @@
       </c>
       <c r="R37" s="8">
         <f t="shared" si="3"/>
-        <v>-8.6382721639824069</v>
+        <v>-8.6925039620867874</v>
       </c>
       <c r="S37" s="11">
-        <v>2.2999999999999999E-9</v>
+        <v>2.0299999999999998E-9</v>
       </c>
       <c r="T37" s="8">
         <f t="shared" si="4"/>
-        <v>2.2999999999999991E-9</v>
+        <v>2.0299999999999949E-9</v>
       </c>
       <c r="U37" s="11">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.963083675318166E-24</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="19" x14ac:dyDescent="0.25">
@@ -40078,7 +40207,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection sqref="A1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40135,7 +40264,7 @@
         <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G2" t="s">
         <v>152</v>
@@ -40164,7 +40293,7 @@
         <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G3" t="s">
         <v>152</v>
@@ -40179,4 +40308,199 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C4E09B-D435-324A-93D9-F2E66BB18A48}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2">
+        <v>40.359423302858701</v>
+      </c>
+      <c r="D2">
+        <v>-111.813765015565</v>
+      </c>
+      <c r="E2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="28">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3">
+        <v>40.359423302858701</v>
+      </c>
+      <c r="D3">
+        <v>-111.813765015565</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4">
+        <v>40.359423302858701</v>
+      </c>
+      <c r="D4">
+        <v>-111.813765015565</v>
+      </c>
+      <c r="E4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="28">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5">
+        <v>40.359423302858701</v>
+      </c>
+      <c r="D5">
+        <v>-111.813765015565</v>
+      </c>
+      <c r="E5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="28">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6">
+        <v>40.359423302858701</v>
+      </c>
+      <c r="D6">
+        <v>-111.813765015565</v>
+      </c>
+      <c r="E6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="28">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ref docs on gw infiltration
</commit_message>
<xml_diff>
--- a/conc_data.xlsx
+++ b/conc_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenelson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/python_projects/adsolve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2EC9AB-EE5A-D64E-ACDB-9A08949C5DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197EC799-88D8-0F40-8532-45341872BA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28600" windowHeight="18560" activeTab="5" xr2:uid="{B672A836-5648-D342-817E-0FAB6C4978C8}"/>
+    <workbookView xWindow="22920" yWindow="3440" windowWidth="39880" windowHeight="19740" activeTab="2" xr2:uid="{B672A836-5648-D342-817E-0FAB6C4978C8}"/>
   </bookViews>
   <sheets>
     <sheet name="TSSD" sheetId="1" r:id="rId1"/>
@@ -19835,15 +19835,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>577273</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>69273</xdr:rowOff>
+      <xdr:colOff>611910</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>104486</xdr:colOff>
+      <xdr:colOff>139123</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>45605</xdr:rowOff>
+      <xdr:rowOff>184151</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37495,7 +37495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A09E69-E6D4-CC4C-8A80-256D255F91E4}">
   <dimension ref="A1:AL30"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="R2" sqref="R2:R27"/>
     </sheetView>
   </sheetViews>
@@ -40314,7 +40314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C4E09B-D435-324A-93D9-F2E66BB18A48}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>

</xml_diff>